<commit_message>
Deploying to gh-pages from  @ b104afd3c585f18d11d4412f9c0d0e8a5dcb99f3 🚀
</commit_message>
<xml_diff>
--- a/assets/excel/2022_5-2-2.xlsx
+++ b/assets/excel/2022_5-2-2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\Hannover\Dez15-Uebergreifende-Analysen\Projekte\Integrationsmonitoring\github\MT_Site\assets\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A285C03-FFAA-4D49-B1D1-EAD70B281546}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70AF62A6-5C57-450A-AA53-1CDA9807DCC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" xr2:uid="{D78F4DFF-A3F7-4D02-ACE9-C520BEFE96A8}"/>
   </bookViews>
@@ -1058,9 +1058,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12F353FB-E6B2-4122-8FD3-146998CA49AF}">
   <dimension ref="B1:CC72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>